<commit_message>
why does this exist
</commit_message>
<xml_diff>
--- a/Data/new data.xlsx
+++ b/Data/new data.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/3e2a06d20bd816c4/Documents/GitHub/project-1/Data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="234" documentId="11_F25DC773A252ABDACC104838C11F52DE5BDE58E9" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{67A1B621-0D6C-477D-805E-1D7CE603FFF1}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="8_{DBB45A7C-EDFE-4743-B8CF-65C982B0DCDB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="22780" windowHeight="15260" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -20,6 +20,7 @@
     <sheet name="Princeton" sheetId="4" r:id="rId5"/>
     <sheet name="Steve Hunt" sheetId="5" r:id="rId6"/>
     <sheet name="Carroll Teaching" sheetId="6" r:id="rId7"/>
+    <sheet name="Links" sheetId="8" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191028"/>
   <extLst>
@@ -96,7 +97,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6598" uniqueCount="1134">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="7042" uniqueCount="1183">
   <si>
     <t>Rk</t>
   </si>
@@ -3498,6 +3499,153 @@
   </si>
   <si>
     <t>Sissy, Sizi Zhang</t>
+  </si>
+  <si>
+    <t>CC SADU</t>
+  </si>
+  <si>
+    <t>CC</t>
+  </si>
+  <si>
+    <t>CC LEMC</t>
+  </si>
+  <si>
+    <t>SEA HEBE</t>
+  </si>
+  <si>
+    <t>SEA</t>
+  </si>
+  <si>
+    <t>LCC TOMO</t>
+  </si>
+  <si>
+    <t>LCC</t>
+  </si>
+  <si>
+    <t>CC THTO</t>
+  </si>
+  <si>
+    <t>SEA DOBE</t>
+  </si>
+  <si>
+    <t>WILL DODI</t>
+  </si>
+  <si>
+    <t>WILL</t>
+  </si>
+  <si>
+    <t>CC LIWI</t>
+  </si>
+  <si>
+    <t>CC SAME</t>
+  </si>
+  <si>
+    <t>LCC FICH</t>
+  </si>
+  <si>
+    <t>WILL KECH</t>
+  </si>
+  <si>
+    <t>LIN JOSM</t>
+  </si>
+  <si>
+    <t>LIN</t>
+  </si>
+  <si>
+    <t>WILL TRCO</t>
+  </si>
+  <si>
+    <t>CC MOST</t>
+  </si>
+  <si>
+    <t>SEA JAPI</t>
+  </si>
+  <si>
+    <t>CC JEBA</t>
+  </si>
+  <si>
+    <t>CC FRHA</t>
+  </si>
+  <si>
+    <t>CC KECR</t>
+  </si>
+  <si>
+    <t>SEA KHNA</t>
+  </si>
+  <si>
+    <t>CC ORWI</t>
+  </si>
+  <si>
+    <t>SEA DUSL</t>
+  </si>
+  <si>
+    <t>LCC KOSH</t>
+  </si>
+  <si>
+    <t>CC SAPO</t>
+  </si>
+  <si>
+    <t>SEA BRGE</t>
+  </si>
+  <si>
+    <t>1=</t>
+  </si>
+  <si>
+    <t>4=</t>
+  </si>
+  <si>
+    <t>Charles Said</t>
+  </si>
+  <si>
+    <t>Maltin TOcani</t>
+  </si>
+  <si>
+    <t>13=</t>
+  </si>
+  <si>
+    <t>Leah Melvin</t>
+  </si>
+  <si>
+    <t>Ethan Smith</t>
+  </si>
+  <si>
+    <t>15=</t>
+  </si>
+  <si>
+    <t>Merren Troll</t>
+  </si>
+  <si>
+    <t>19=</t>
+  </si>
+  <si>
+    <t>Ronan Cole</t>
+  </si>
+  <si>
+    <t>Emily Mowat</t>
+  </si>
+  <si>
+    <t>Katy Keim</t>
+  </si>
+  <si>
+    <t>33=</t>
+  </si>
+  <si>
+    <t>Na&amp;#x27;ama Shuall</t>
+  </si>
+  <si>
+    <t>Kayden Crozier</t>
+  </si>
+  <si>
+    <t>Madison Kollar</t>
+  </si>
+  <si>
+    <t>39=</t>
+  </si>
+  <si>
+    <t>45=</t>
+  </si>
+  <si>
+    <t>Sophie Portmann</t>
   </si>
 </sst>
 </file>
@@ -3852,21 +4000,2468 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B7403276-E188-471B-8F2F-6D081A417FF0}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:P49"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K26" sqref="K26"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:16" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
-        <v>537</v>
+        <v>0</v>
+      </c>
+      <c r="B1" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" t="s">
+        <v>3</v>
+      </c>
+      <c r="D1" t="s">
+        <v>1</v>
+      </c>
+      <c r="E1" t="s">
+        <v>4</v>
+      </c>
+      <c r="F1" t="s">
+        <v>5</v>
+      </c>
+      <c r="G1" t="s">
+        <v>6</v>
+      </c>
+      <c r="H1" t="s">
+        <v>7</v>
+      </c>
+      <c r="I1" t="s">
+        <v>8</v>
+      </c>
+      <c r="J1" t="s">
+        <v>9</v>
+      </c>
+      <c r="K1" t="s">
+        <v>10</v>
+      </c>
+      <c r="L1" t="s">
+        <v>11</v>
+      </c>
+      <c r="M1" t="s">
+        <v>12</v>
+      </c>
+      <c r="N1" t="s">
+        <v>14</v>
+      </c>
+      <c r="O1" t="s">
+        <v>15</v>
+      </c>
+      <c r="P1" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="2" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B2" t="s">
+        <v>105</v>
+      </c>
+      <c r="C2" t="s">
+        <v>21</v>
+      </c>
+      <c r="D2" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E2" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F2" t="s">
+        <v>374</v>
+      </c>
+      <c r="G2">
+        <v>77</v>
+      </c>
+      <c r="H2" t="s">
+        <v>374</v>
+      </c>
+      <c r="I2">
+        <v>79</v>
+      </c>
+      <c r="J2" t="s">
+        <v>374</v>
+      </c>
+      <c r="K2">
+        <v>78</v>
+      </c>
+      <c r="L2" t="s">
+        <v>375</v>
+      </c>
+      <c r="M2">
+        <v>80</v>
+      </c>
+      <c r="N2">
+        <v>314</v>
+      </c>
+      <c r="O2">
+        <v>78.5</v>
+      </c>
+      <c r="P2">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="3" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B3" t="s">
+        <v>626</v>
+      </c>
+      <c r="C3" t="s">
+        <v>21</v>
+      </c>
+      <c r="D3" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E3" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F3" t="s">
+        <v>374</v>
+      </c>
+      <c r="G3">
+        <v>80</v>
+      </c>
+      <c r="H3" t="s">
+        <v>377</v>
+      </c>
+      <c r="I3">
+        <v>77</v>
+      </c>
+      <c r="J3" t="s">
+        <v>377</v>
+      </c>
+      <c r="K3">
+        <v>77</v>
+      </c>
+      <c r="L3" t="s">
+        <v>377</v>
+      </c>
+      <c r="M3">
+        <v>80</v>
+      </c>
+      <c r="N3">
+        <v>314</v>
+      </c>
+      <c r="O3">
+        <v>78.5</v>
+      </c>
+      <c r="P3">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="4" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>1163</v>
+      </c>
+      <c r="B4" t="s">
+        <v>107</v>
+      </c>
+      <c r="C4" t="s">
+        <v>21</v>
+      </c>
+      <c r="D4" t="s">
+        <v>1136</v>
+      </c>
+      <c r="E4" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F4" t="s">
+        <v>374</v>
+      </c>
+      <c r="G4">
+        <v>79</v>
+      </c>
+      <c r="H4" t="s">
+        <v>377</v>
+      </c>
+      <c r="I4">
+        <v>78</v>
+      </c>
+      <c r="J4" t="s">
+        <v>377</v>
+      </c>
+      <c r="K4">
+        <v>76</v>
+      </c>
+      <c r="L4" t="s">
+        <v>377</v>
+      </c>
+      <c r="M4">
+        <v>81</v>
+      </c>
+      <c r="N4">
+        <v>314</v>
+      </c>
+      <c r="O4">
+        <v>78.5</v>
+      </c>
+      <c r="P4">
+        <v>1.8</v>
+      </c>
+    </row>
+    <row r="5" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B5" t="s">
+        <v>1165</v>
+      </c>
+      <c r="C5" t="s">
+        <v>21</v>
+      </c>
+      <c r="D5" t="s">
+        <v>1134</v>
+      </c>
+      <c r="E5" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F5" t="s">
+        <v>374</v>
+      </c>
+      <c r="G5">
+        <v>77</v>
+      </c>
+      <c r="H5" t="s">
+        <v>374</v>
+      </c>
+      <c r="I5">
+        <v>78</v>
+      </c>
+      <c r="J5" t="s">
+        <v>374</v>
+      </c>
+      <c r="K5">
+        <v>77</v>
+      </c>
+      <c r="L5" t="s">
+        <v>375</v>
+      </c>
+      <c r="M5">
+        <v>80</v>
+      </c>
+      <c r="N5">
+        <v>312</v>
+      </c>
+      <c r="O5">
+        <v>78</v>
+      </c>
+      <c r="P5">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="6" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B6" t="s">
+        <v>115</v>
+      </c>
+      <c r="C6" t="s">
+        <v>21</v>
+      </c>
+      <c r="D6" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E6" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F6" t="s">
+        <v>374</v>
+      </c>
+      <c r="G6">
+        <v>77</v>
+      </c>
+      <c r="H6" t="s">
+        <v>377</v>
+      </c>
+      <c r="I6">
+        <v>76</v>
+      </c>
+      <c r="J6" t="s">
+        <v>374</v>
+      </c>
+      <c r="K6">
+        <v>80</v>
+      </c>
+      <c r="L6" t="s">
+        <v>376</v>
+      </c>
+      <c r="M6">
+        <v>79</v>
+      </c>
+      <c r="N6">
+        <v>312</v>
+      </c>
+      <c r="O6">
+        <v>78</v>
+      </c>
+      <c r="P6">
+        <v>1.58</v>
+      </c>
+    </row>
+    <row r="7" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A7">
+        <v>6</v>
+      </c>
+      <c r="B7" t="s">
+        <v>278</v>
+      </c>
+      <c r="C7" t="s">
+        <v>21</v>
+      </c>
+      <c r="D7" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E7" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F7" t="s">
+        <v>374</v>
+      </c>
+      <c r="G7">
+        <v>78</v>
+      </c>
+      <c r="H7" t="s">
+        <v>374</v>
+      </c>
+      <c r="I7">
+        <v>76</v>
+      </c>
+      <c r="J7" t="s">
+        <v>376</v>
+      </c>
+      <c r="K7">
+        <v>74</v>
+      </c>
+      <c r="L7" t="s">
+        <v>374</v>
+      </c>
+      <c r="M7">
+        <v>82</v>
+      </c>
+      <c r="N7">
+        <v>310</v>
+      </c>
+      <c r="O7">
+        <v>77.5</v>
+      </c>
+      <c r="P7">
+        <v>2.96</v>
+      </c>
+    </row>
+    <row r="8" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A8" t="s">
+        <v>436</v>
+      </c>
+      <c r="B8" t="s">
+        <v>136</v>
+      </c>
+      <c r="C8" t="s">
+        <v>27</v>
+      </c>
+      <c r="D8" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E8" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F8" t="s">
+        <v>375</v>
+      </c>
+      <c r="G8">
+        <v>77</v>
+      </c>
+      <c r="H8" t="s">
+        <v>375</v>
+      </c>
+      <c r="I8">
+        <v>78</v>
+      </c>
+      <c r="J8" t="s">
+        <v>374</v>
+      </c>
+      <c r="K8">
+        <v>77</v>
+      </c>
+      <c r="L8" t="s">
+        <v>377</v>
+      </c>
+      <c r="M8">
+        <v>77</v>
+      </c>
+      <c r="N8">
+        <v>309</v>
+      </c>
+      <c r="O8">
+        <v>77.25</v>
+      </c>
+      <c r="P8">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="9" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A9" t="s">
+        <v>436</v>
+      </c>
+      <c r="B9" t="s">
+        <v>116</v>
+      </c>
+      <c r="C9" t="s">
+        <v>21</v>
+      </c>
+      <c r="D9" t="s">
+        <v>1141</v>
+      </c>
+      <c r="E9" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F9" t="s">
+        <v>374</v>
+      </c>
+      <c r="G9">
+        <v>77</v>
+      </c>
+      <c r="H9" t="s">
+        <v>377</v>
+      </c>
+      <c r="I9">
+        <v>75</v>
+      </c>
+      <c r="J9" t="s">
+        <v>374</v>
+      </c>
+      <c r="K9">
+        <v>79</v>
+      </c>
+      <c r="L9" t="s">
+        <v>376</v>
+      </c>
+      <c r="M9">
+        <v>78</v>
+      </c>
+      <c r="N9">
+        <v>309</v>
+      </c>
+      <c r="O9">
+        <v>77.25</v>
+      </c>
+      <c r="P9">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="10" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>436</v>
+      </c>
+      <c r="B10" t="s">
+        <v>1166</v>
+      </c>
+      <c r="C10" t="s">
+        <v>21</v>
+      </c>
+      <c r="D10" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E10" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F10" t="s">
+        <v>377</v>
+      </c>
+      <c r="G10">
+        <v>77</v>
+      </c>
+      <c r="H10" t="s">
+        <v>375</v>
+      </c>
+      <c r="I10">
+        <v>75</v>
+      </c>
+      <c r="J10" t="s">
+        <v>374</v>
+      </c>
+      <c r="K10">
+        <v>78</v>
+      </c>
+      <c r="L10" t="s">
+        <v>374</v>
+      </c>
+      <c r="M10">
+        <v>79</v>
+      </c>
+      <c r="N10">
+        <v>309</v>
+      </c>
+      <c r="O10">
+        <v>77.25</v>
+      </c>
+      <c r="P10">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="11" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>436</v>
+      </c>
+      <c r="B11" t="s">
+        <v>279</v>
+      </c>
+      <c r="C11" t="s">
+        <v>21</v>
+      </c>
+      <c r="D11" t="s">
+        <v>1137</v>
+      </c>
+      <c r="E11" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F11" t="s">
+        <v>374</v>
+      </c>
+      <c r="G11">
+        <v>78</v>
+      </c>
+      <c r="H11" t="s">
+        <v>374</v>
+      </c>
+      <c r="I11">
+        <v>77</v>
+      </c>
+      <c r="J11" t="s">
+        <v>376</v>
+      </c>
+      <c r="K11">
+        <v>73</v>
+      </c>
+      <c r="L11" t="s">
+        <v>374</v>
+      </c>
+      <c r="M11">
+        <v>81</v>
+      </c>
+      <c r="N11">
+        <v>309</v>
+      </c>
+      <c r="O11">
+        <v>77.25</v>
+      </c>
+      <c r="P11">
+        <v>2.86</v>
+      </c>
+    </row>
+    <row r="12" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A12">
+        <v>11</v>
+      </c>
+      <c r="B12" t="s">
+        <v>480</v>
+      </c>
+      <c r="C12" t="s">
+        <v>21</v>
+      </c>
+      <c r="D12" t="s">
+        <v>1139</v>
+      </c>
+      <c r="E12" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F12" t="s">
+        <v>377</v>
+      </c>
+      <c r="G12">
+        <v>78</v>
+      </c>
+      <c r="H12" t="s">
+        <v>375</v>
+      </c>
+      <c r="I12">
+        <v>75</v>
+      </c>
+      <c r="J12" t="s">
+        <v>374</v>
+      </c>
+      <c r="K12">
+        <v>77</v>
+      </c>
+      <c r="L12" t="s">
+        <v>374</v>
+      </c>
+      <c r="M12">
+        <v>78</v>
+      </c>
+      <c r="N12">
+        <v>308</v>
+      </c>
+      <c r="O12">
+        <v>77</v>
+      </c>
+      <c r="P12">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="13" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A13">
+        <v>12</v>
+      </c>
+      <c r="B13" t="s">
+        <v>354</v>
+      </c>
+      <c r="C13" t="s">
+        <v>21</v>
+      </c>
+      <c r="D13" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E13" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F13" t="s">
+        <v>377</v>
+      </c>
+      <c r="G13">
+        <v>78</v>
+      </c>
+      <c r="H13" t="s">
+        <v>375</v>
+      </c>
+      <c r="I13">
+        <v>75</v>
+      </c>
+      <c r="J13" t="s">
+        <v>377</v>
+      </c>
+      <c r="K13">
+        <v>76</v>
+      </c>
+      <c r="L13" t="s">
+        <v>374</v>
+      </c>
+      <c r="M13">
+        <v>78</v>
+      </c>
+      <c r="N13">
+        <v>307</v>
+      </c>
+      <c r="O13">
+        <v>76.75</v>
+      </c>
+      <c r="P13">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="14" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B14" t="s">
+        <v>1168</v>
+      </c>
+      <c r="C14" t="s">
+        <v>27</v>
+      </c>
+      <c r="D14" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E14" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F14" t="s">
+        <v>374</v>
+      </c>
+      <c r="G14">
+        <v>76</v>
+      </c>
+      <c r="H14" t="s">
+        <v>376</v>
+      </c>
+      <c r="I14">
+        <v>76</v>
+      </c>
+      <c r="J14" t="s">
+        <v>374</v>
+      </c>
+      <c r="K14">
+        <v>78</v>
+      </c>
+      <c r="L14" t="s">
+        <v>375</v>
+      </c>
+      <c r="M14">
+        <v>76</v>
+      </c>
+      <c r="N14">
+        <v>306</v>
+      </c>
+      <c r="O14">
+        <v>76.5</v>
+      </c>
+      <c r="P14">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="15" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
+        <v>1167</v>
+      </c>
+      <c r="B15" t="s">
+        <v>1169</v>
+      </c>
+      <c r="C15" t="s">
+        <v>21</v>
+      </c>
+      <c r="D15" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E15" t="s">
+        <v>1150</v>
+      </c>
+      <c r="F15" t="s">
+        <v>374</v>
+      </c>
+      <c r="G15">
+        <v>77</v>
+      </c>
+      <c r="H15" t="s">
+        <v>375</v>
+      </c>
+      <c r="I15">
+        <v>77</v>
+      </c>
+      <c r="J15" t="s">
+        <v>375</v>
+      </c>
+      <c r="K15">
+        <v>77</v>
+      </c>
+      <c r="L15" t="s">
+        <v>375</v>
+      </c>
+      <c r="M15">
+        <v>75</v>
+      </c>
+      <c r="N15">
+        <v>306</v>
+      </c>
+      <c r="O15">
+        <v>76.5</v>
+      </c>
+      <c r="P15">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="16" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A16" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B16" t="s">
+        <v>110</v>
+      </c>
+      <c r="C16" t="s">
+        <v>27</v>
+      </c>
+      <c r="D16" t="s">
+        <v>1146</v>
+      </c>
+      <c r="E16" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F16" t="s">
+        <v>374</v>
+      </c>
+      <c r="G16">
+        <v>76</v>
+      </c>
+      <c r="H16" t="s">
+        <v>376</v>
+      </c>
+      <c r="I16">
+        <v>76</v>
+      </c>
+      <c r="J16" t="s">
+        <v>374</v>
+      </c>
+      <c r="K16">
+        <v>78</v>
+      </c>
+      <c r="L16" t="s">
+        <v>375</v>
+      </c>
+      <c r="M16">
+        <v>75</v>
+      </c>
+      <c r="N16">
+        <v>305</v>
+      </c>
+      <c r="O16">
+        <v>76.25</v>
+      </c>
+      <c r="P16">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="17" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B17" t="s">
+        <v>686</v>
+      </c>
+      <c r="C17" t="s">
+        <v>27</v>
+      </c>
+      <c r="D17" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E17" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F17" t="s">
+        <v>376</v>
+      </c>
+      <c r="G17">
+        <v>76</v>
+      </c>
+      <c r="H17" t="s">
+        <v>375</v>
+      </c>
+      <c r="I17">
+        <v>75</v>
+      </c>
+      <c r="J17" t="s">
+        <v>374</v>
+      </c>
+      <c r="K17">
+        <v>77</v>
+      </c>
+      <c r="L17" t="s">
+        <v>374</v>
+      </c>
+      <c r="M17">
+        <v>77</v>
+      </c>
+      <c r="N17">
+        <v>305</v>
+      </c>
+      <c r="O17">
+        <v>76.25</v>
+      </c>
+      <c r="P17">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="18" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A18" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B18" t="s">
+        <v>1171</v>
+      </c>
+      <c r="C18" t="s">
+        <v>27</v>
+      </c>
+      <c r="D18" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E18" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F18" t="s">
+        <v>377</v>
+      </c>
+      <c r="G18">
+        <v>77</v>
+      </c>
+      <c r="H18" t="s">
+        <v>377</v>
+      </c>
+      <c r="I18">
+        <v>75</v>
+      </c>
+      <c r="J18" t="s">
+        <v>377</v>
+      </c>
+      <c r="K18">
+        <v>78</v>
+      </c>
+      <c r="L18" t="s">
+        <v>376</v>
+      </c>
+      <c r="M18">
+        <v>75</v>
+      </c>
+      <c r="N18">
+        <v>305</v>
+      </c>
+      <c r="O18">
+        <v>76.25</v>
+      </c>
+      <c r="P18">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="19" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
+        <v>1170</v>
+      </c>
+      <c r="B19" t="s">
+        <v>270</v>
+      </c>
+      <c r="C19" t="s">
+        <v>21</v>
+      </c>
+      <c r="D19" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E19" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F19" t="s">
+        <v>377</v>
+      </c>
+      <c r="G19">
+        <v>77</v>
+      </c>
+      <c r="H19" t="s">
+        <v>374</v>
+      </c>
+      <c r="I19">
+        <v>77</v>
+      </c>
+      <c r="J19" t="s">
+        <v>375</v>
+      </c>
+      <c r="K19">
+        <v>75</v>
+      </c>
+      <c r="L19" t="s">
+        <v>377</v>
+      </c>
+      <c r="M19">
+        <v>76</v>
+      </c>
+      <c r="N19">
+        <v>305</v>
+      </c>
+      <c r="O19">
+        <v>76.25</v>
+      </c>
+      <c r="P19">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="20" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A20" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B20" t="s">
+        <v>164</v>
+      </c>
+      <c r="C20" t="s">
+        <v>21</v>
+      </c>
+      <c r="D20" t="s">
+        <v>1149</v>
+      </c>
+      <c r="E20" t="s">
+        <v>1150</v>
+      </c>
+      <c r="F20" t="s">
+        <v>374</v>
+      </c>
+      <c r="G20">
+        <v>77</v>
+      </c>
+      <c r="H20" t="s">
+        <v>375</v>
+      </c>
+      <c r="I20">
+        <v>76</v>
+      </c>
+      <c r="J20" t="s">
+        <v>375</v>
+      </c>
+      <c r="K20">
+        <v>76</v>
+      </c>
+      <c r="L20" t="s">
+        <v>375</v>
+      </c>
+      <c r="M20">
+        <v>75</v>
+      </c>
+      <c r="N20">
+        <v>304</v>
+      </c>
+      <c r="O20">
+        <v>76</v>
+      </c>
+      <c r="P20">
+        <v>0.71</v>
+      </c>
+    </row>
+    <row r="21" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>1172</v>
+      </c>
+      <c r="B21" t="s">
+        <v>268</v>
+      </c>
+      <c r="C21" t="s">
+        <v>21</v>
+      </c>
+      <c r="D21" t="s">
+        <v>1142</v>
+      </c>
+      <c r="E21" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F21" t="s">
+        <v>377</v>
+      </c>
+      <c r="G21">
+        <v>76</v>
+      </c>
+      <c r="H21" t="s">
+        <v>374</v>
+      </c>
+      <c r="I21">
+        <v>76</v>
+      </c>
+      <c r="J21" t="s">
+        <v>375</v>
+      </c>
+      <c r="K21">
+        <v>74</v>
+      </c>
+      <c r="L21" t="s">
+        <v>377</v>
+      </c>
+      <c r="M21">
+        <v>78</v>
+      </c>
+      <c r="N21">
+        <v>304</v>
+      </c>
+      <c r="O21">
+        <v>76</v>
+      </c>
+      <c r="P21">
+        <v>1.41</v>
+      </c>
+    </row>
+    <row r="22" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>113</v>
+      </c>
+      <c r="B22" t="s">
+        <v>629</v>
+      </c>
+      <c r="C22" t="s">
+        <v>27</v>
+      </c>
+      <c r="D22" t="s">
+        <v>1145</v>
+      </c>
+      <c r="E22" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F22" t="s">
+        <v>375</v>
+      </c>
+      <c r="G22">
+        <v>76</v>
+      </c>
+      <c r="H22" t="s">
+        <v>375</v>
+      </c>
+      <c r="I22">
+        <v>76</v>
+      </c>
+      <c r="J22" t="s">
+        <v>374</v>
+      </c>
+      <c r="K22">
+        <v>75</v>
+      </c>
+      <c r="L22" t="s">
+        <v>377</v>
+      </c>
+      <c r="M22">
+        <v>76</v>
+      </c>
+      <c r="N22">
+        <v>303</v>
+      </c>
+      <c r="O22">
+        <v>75.75</v>
+      </c>
+      <c r="P22">
+        <v>0.43</v>
+      </c>
+    </row>
+    <row r="23" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A23" t="s">
+        <v>113</v>
+      </c>
+      <c r="B23" t="s">
+        <v>1173</v>
+      </c>
+      <c r="C23" t="s">
+        <v>27</v>
+      </c>
+      <c r="D23" t="s">
+        <v>1151</v>
+      </c>
+      <c r="E23" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F23" t="s">
+        <v>377</v>
+      </c>
+      <c r="G23">
+        <v>75</v>
+      </c>
+      <c r="H23" t="s">
+        <v>377</v>
+      </c>
+      <c r="I23">
+        <v>76</v>
+      </c>
+      <c r="J23" t="s">
+        <v>377</v>
+      </c>
+      <c r="K23">
+        <v>77</v>
+      </c>
+      <c r="L23" t="s">
+        <v>376</v>
+      </c>
+      <c r="M23">
+        <v>75</v>
+      </c>
+      <c r="N23">
+        <v>303</v>
+      </c>
+      <c r="O23">
+        <v>75.75</v>
+      </c>
+      <c r="P23">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="24" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B24" t="s">
+        <v>667</v>
+      </c>
+      <c r="C24" t="s">
+        <v>21</v>
+      </c>
+      <c r="D24" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E24" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F24" t="s">
+        <v>377</v>
+      </c>
+      <c r="G24">
+        <v>77</v>
+      </c>
+      <c r="H24" t="s">
+        <v>376</v>
+      </c>
+      <c r="I24">
+        <v>75</v>
+      </c>
+      <c r="J24" t="s">
+        <v>375</v>
+      </c>
+      <c r="K24">
+        <v>75</v>
+      </c>
+      <c r="L24" t="s">
+        <v>377</v>
+      </c>
+      <c r="M24">
+        <v>76</v>
+      </c>
+      <c r="N24">
+        <v>303</v>
+      </c>
+      <c r="O24">
+        <v>75.75</v>
+      </c>
+      <c r="P24">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="25" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>113</v>
+      </c>
+      <c r="B25" t="s">
+        <v>1174</v>
+      </c>
+      <c r="C25" t="s">
+        <v>21</v>
+      </c>
+      <c r="D25" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E25" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F25" t="s">
+        <v>375</v>
+      </c>
+      <c r="G25">
+        <v>75</v>
+      </c>
+      <c r="H25" t="s">
+        <v>374</v>
+      </c>
+      <c r="I25">
+        <v>78</v>
+      </c>
+      <c r="J25" t="s">
+        <v>376</v>
+      </c>
+      <c r="K25">
+        <v>76</v>
+      </c>
+      <c r="L25" t="s">
+        <v>375</v>
+      </c>
+      <c r="M25">
+        <v>74</v>
+      </c>
+      <c r="N25">
+        <v>303</v>
+      </c>
+      <c r="O25">
+        <v>75.75</v>
+      </c>
+      <c r="P25">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="26" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>113</v>
+      </c>
+      <c r="B26" t="s">
+        <v>108</v>
+      </c>
+      <c r="C26" t="s">
+        <v>21</v>
+      </c>
+      <c r="D26" t="s">
+        <v>1152</v>
+      </c>
+      <c r="E26" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F26" t="s">
+        <v>375</v>
+      </c>
+      <c r="G26">
+        <v>75</v>
+      </c>
+      <c r="H26" t="s">
+        <v>374</v>
+      </c>
+      <c r="I26">
+        <v>78</v>
+      </c>
+      <c r="J26" t="s">
+        <v>376</v>
+      </c>
+      <c r="K26">
+        <v>76</v>
+      </c>
+      <c r="L26" t="s">
+        <v>375</v>
+      </c>
+      <c r="M26">
+        <v>74</v>
+      </c>
+      <c r="N26">
+        <v>303</v>
+      </c>
+      <c r="O26">
+        <v>75.75</v>
+      </c>
+      <c r="P26">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="27" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>113</v>
+      </c>
+      <c r="B27" t="s">
+        <v>281</v>
+      </c>
+      <c r="C27" t="s">
+        <v>27</v>
+      </c>
+      <c r="D27" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E27" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F27" t="s">
+        <v>375</v>
+      </c>
+      <c r="G27">
+        <v>75</v>
+      </c>
+      <c r="H27" t="s">
+        <v>374</v>
+      </c>
+      <c r="I27">
+        <v>80</v>
+      </c>
+      <c r="J27" t="s">
+        <v>376</v>
+      </c>
+      <c r="K27">
+        <v>73</v>
+      </c>
+      <c r="L27" t="s">
+        <v>375</v>
+      </c>
+      <c r="M27">
+        <v>75</v>
+      </c>
+      <c r="N27">
+        <v>303</v>
+      </c>
+      <c r="O27">
+        <v>75.75</v>
+      </c>
+      <c r="P27">
+        <v>2.59</v>
+      </c>
+    </row>
+    <row r="28" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>113</v>
+      </c>
+      <c r="B28" t="s">
+        <v>357</v>
+      </c>
+      <c r="C28" t="s">
+        <v>21</v>
+      </c>
+      <c r="D28" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E28" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F28" t="s">
+        <v>375</v>
+      </c>
+      <c r="G28">
+        <v>75</v>
+      </c>
+      <c r="H28" t="s">
+        <v>375</v>
+      </c>
+      <c r="I28">
+        <v>76</v>
+      </c>
+      <c r="J28" t="s">
+        <v>377</v>
+      </c>
+      <c r="K28">
+        <v>77</v>
+      </c>
+      <c r="L28" t="s">
+        <v>374</v>
+      </c>
+      <c r="M28">
+        <v>75</v>
+      </c>
+      <c r="N28">
+        <v>303</v>
+      </c>
+      <c r="O28">
+        <v>75.75</v>
+      </c>
+      <c r="P28">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="29" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>463</v>
+      </c>
+      <c r="B29" t="s">
+        <v>694</v>
+      </c>
+      <c r="C29" t="s">
+        <v>27</v>
+      </c>
+      <c r="D29" t="s">
+        <v>1147</v>
+      </c>
+      <c r="E29" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F29" t="s">
+        <v>376</v>
+      </c>
+      <c r="G29">
+        <v>76</v>
+      </c>
+      <c r="H29" t="s">
+        <v>375</v>
+      </c>
+      <c r="I29">
+        <v>74</v>
+      </c>
+      <c r="J29" t="s">
+        <v>374</v>
+      </c>
+      <c r="K29">
+        <v>76</v>
+      </c>
+      <c r="L29" t="s">
+        <v>374</v>
+      </c>
+      <c r="M29">
+        <v>76</v>
+      </c>
+      <c r="N29">
+        <v>302</v>
+      </c>
+      <c r="O29">
+        <v>75.5</v>
+      </c>
+      <c r="P29">
+        <v>0.87</v>
+      </c>
+    </row>
+    <row r="30" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>463</v>
+      </c>
+      <c r="B30" t="s">
+        <v>666</v>
+      </c>
+      <c r="C30" t="s">
+        <v>27</v>
+      </c>
+      <c r="D30" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E30" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F30" t="s">
+        <v>375</v>
+      </c>
+      <c r="G30">
+        <v>75</v>
+      </c>
+      <c r="H30" t="s">
+        <v>377</v>
+      </c>
+      <c r="I30">
+        <v>78</v>
+      </c>
+      <c r="J30" t="s">
+        <v>375</v>
+      </c>
+      <c r="K30">
+        <v>75</v>
+      </c>
+      <c r="L30" t="s">
+        <v>376</v>
+      </c>
+      <c r="M30">
+        <v>74</v>
+      </c>
+      <c r="N30">
+        <v>302</v>
+      </c>
+      <c r="O30">
+        <v>75.5</v>
+      </c>
+      <c r="P30">
+        <v>1.5</v>
+      </c>
+    </row>
+    <row r="31" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>463</v>
+      </c>
+      <c r="B31" t="s">
+        <v>1175</v>
+      </c>
+      <c r="C31" t="s">
+        <v>21</v>
+      </c>
+      <c r="D31" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E31" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F31" t="s">
+        <v>376</v>
+      </c>
+      <c r="G31">
+        <v>75</v>
+      </c>
+      <c r="H31" t="s">
+        <v>376</v>
+      </c>
+      <c r="I31">
+        <v>76</v>
+      </c>
+      <c r="J31" t="s">
+        <v>377</v>
+      </c>
+      <c r="K31">
+        <v>76</v>
+      </c>
+      <c r="L31" t="s">
+        <v>377</v>
+      </c>
+      <c r="M31">
+        <v>75</v>
+      </c>
+      <c r="N31">
+        <v>302</v>
+      </c>
+      <c r="O31">
+        <v>75.5</v>
+      </c>
+      <c r="P31">
+        <v>0.5</v>
+      </c>
+    </row>
+    <row r="32" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>463</v>
+      </c>
+      <c r="B32" t="s">
+        <v>348</v>
+      </c>
+      <c r="C32" t="s">
+        <v>21</v>
+      </c>
+      <c r="D32" t="s">
+        <v>1143</v>
+      </c>
+      <c r="E32" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F32" t="s">
+        <v>377</v>
+      </c>
+      <c r="G32">
+        <v>76</v>
+      </c>
+      <c r="H32" t="s">
+        <v>375</v>
+      </c>
+      <c r="I32">
+        <v>74</v>
+      </c>
+      <c r="J32" t="s">
+        <v>377</v>
+      </c>
+      <c r="K32">
+        <v>75</v>
+      </c>
+      <c r="L32" t="s">
+        <v>374</v>
+      </c>
+      <c r="M32">
+        <v>77</v>
+      </c>
+      <c r="N32">
+        <v>302</v>
+      </c>
+      <c r="O32">
+        <v>75.5</v>
+      </c>
+      <c r="P32">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="33" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>463</v>
+      </c>
+      <c r="B33" t="s">
+        <v>347</v>
+      </c>
+      <c r="C33" t="s">
+        <v>21</v>
+      </c>
+      <c r="D33" t="s">
+        <v>1148</v>
+      </c>
+      <c r="E33" t="s">
+        <v>1144</v>
+      </c>
+      <c r="F33" t="s">
+        <v>375</v>
+      </c>
+      <c r="G33">
+        <v>74</v>
+      </c>
+      <c r="H33" t="s">
+        <v>375</v>
+      </c>
+      <c r="I33">
+        <v>77</v>
+      </c>
+      <c r="J33" t="s">
+        <v>377</v>
+      </c>
+      <c r="K33">
+        <v>76</v>
+      </c>
+      <c r="L33" t="s">
+        <v>374</v>
+      </c>
+      <c r="M33">
+        <v>75</v>
+      </c>
+      <c r="N33">
+        <v>302</v>
+      </c>
+      <c r="O33">
+        <v>75.5</v>
+      </c>
+      <c r="P33">
+        <v>1.1200000000000001</v>
+      </c>
+    </row>
+    <row r="34" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B34" t="s">
+        <v>1177</v>
+      </c>
+      <c r="C34" t="s">
+        <v>27</v>
+      </c>
+      <c r="D34" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E34" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F34" t="s">
+        <v>376</v>
+      </c>
+      <c r="G34">
+        <v>75</v>
+      </c>
+      <c r="H34" t="s">
+        <v>377</v>
+      </c>
+      <c r="I34">
+        <v>77</v>
+      </c>
+      <c r="J34" t="s">
+        <v>376</v>
+      </c>
+      <c r="K34">
+        <v>74</v>
+      </c>
+      <c r="L34" t="s">
+        <v>375</v>
+      </c>
+      <c r="M34">
+        <v>75</v>
+      </c>
+      <c r="N34">
+        <v>301</v>
+      </c>
+      <c r="O34">
+        <v>75.25</v>
+      </c>
+      <c r="P34">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="35" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B35" t="s">
+        <v>633</v>
+      </c>
+      <c r="C35" t="s">
+        <v>21</v>
+      </c>
+      <c r="D35" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E35" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F35" t="s">
+        <v>376</v>
+      </c>
+      <c r="G35">
+        <v>74</v>
+      </c>
+      <c r="H35" t="s">
+        <v>374</v>
+      </c>
+      <c r="I35">
+        <v>78</v>
+      </c>
+      <c r="J35" t="s">
+        <v>376</v>
+      </c>
+      <c r="K35">
+        <v>74</v>
+      </c>
+      <c r="L35" t="s">
+        <v>377</v>
+      </c>
+      <c r="M35">
+        <v>75</v>
+      </c>
+      <c r="N35">
+        <v>301</v>
+      </c>
+      <c r="O35">
+        <v>75.25</v>
+      </c>
+      <c r="P35">
+        <v>1.64</v>
+      </c>
+    </row>
+    <row r="36" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B36" t="s">
+        <v>1178</v>
+      </c>
+      <c r="C36" t="s">
+        <v>21</v>
+      </c>
+      <c r="D36" t="s">
+        <v>1156</v>
+      </c>
+      <c r="E36" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F36" t="s">
+        <v>376</v>
+      </c>
+      <c r="G36">
+        <v>73</v>
+      </c>
+      <c r="H36" t="s">
+        <v>376</v>
+      </c>
+      <c r="I36">
+        <v>76</v>
+      </c>
+      <c r="J36" t="s">
+        <v>377</v>
+      </c>
+      <c r="K36">
+        <v>76</v>
+      </c>
+      <c r="L36" t="s">
+        <v>377</v>
+      </c>
+      <c r="M36">
+        <v>76</v>
+      </c>
+      <c r="N36">
+        <v>301</v>
+      </c>
+      <c r="O36">
+        <v>75.25</v>
+      </c>
+      <c r="P36">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="37" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>1176</v>
+      </c>
+      <c r="B37" t="s">
+        <v>658</v>
+      </c>
+      <c r="C37" t="s">
+        <v>21</v>
+      </c>
+      <c r="D37" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E37" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F37" t="s">
+        <v>375</v>
+      </c>
+      <c r="G37">
+        <v>75</v>
+      </c>
+      <c r="H37" t="s">
+        <v>376</v>
+      </c>
+      <c r="I37">
+        <v>74</v>
+      </c>
+      <c r="J37" t="s">
+        <v>376</v>
+      </c>
+      <c r="K37">
+        <v>75</v>
+      </c>
+      <c r="L37" t="s">
+        <v>374</v>
+      </c>
+      <c r="M37">
+        <v>77</v>
+      </c>
+      <c r="N37">
+        <v>301</v>
+      </c>
+      <c r="O37">
+        <v>75.25</v>
+      </c>
+      <c r="P37">
+        <v>1.0900000000000001</v>
+      </c>
+    </row>
+    <row r="38" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>475</v>
+      </c>
+      <c r="B38" t="s">
+        <v>1179</v>
+      </c>
+      <c r="C38" t="s">
+        <v>27</v>
+      </c>
+      <c r="D38" t="s">
+        <v>1160</v>
+      </c>
+      <c r="E38" t="s">
+        <v>1140</v>
+      </c>
+      <c r="F38" t="s">
+        <v>376</v>
+      </c>
+      <c r="G38">
+        <v>74</v>
+      </c>
+      <c r="H38" t="s">
+        <v>377</v>
+      </c>
+      <c r="I38">
+        <v>78</v>
+      </c>
+      <c r="J38" t="s">
+        <v>376</v>
+      </c>
+      <c r="K38">
+        <v>73</v>
+      </c>
+      <c r="L38" t="s">
+        <v>375</v>
+      </c>
+      <c r="M38">
+        <v>75</v>
+      </c>
+      <c r="N38">
+        <v>300</v>
+      </c>
+      <c r="O38">
+        <v>75</v>
+      </c>
+      <c r="P38">
+        <v>1.87</v>
+      </c>
+    </row>
+    <row r="39" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>475</v>
+      </c>
+      <c r="B39" t="s">
+        <v>284</v>
+      </c>
+      <c r="C39" t="s">
+        <v>27</v>
+      </c>
+      <c r="D39" t="s">
+        <v>1157</v>
+      </c>
+      <c r="E39" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F39" t="s">
+        <v>375</v>
+      </c>
+      <c r="G39">
+        <v>74</v>
+      </c>
+      <c r="H39" t="s">
+        <v>377</v>
+      </c>
+      <c r="I39">
+        <v>78</v>
+      </c>
+      <c r="J39" t="s">
+        <v>375</v>
+      </c>
+      <c r="K39">
+        <v>74</v>
+      </c>
+      <c r="L39" t="s">
+        <v>376</v>
+      </c>
+      <c r="M39">
+        <v>74</v>
+      </c>
+      <c r="N39">
+        <v>300</v>
+      </c>
+      <c r="O39">
+        <v>75</v>
+      </c>
+      <c r="P39">
+        <v>1.73</v>
+      </c>
+    </row>
+    <row r="40" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B40" t="s">
+        <v>112</v>
+      </c>
+      <c r="C40" t="s">
+        <v>27</v>
+      </c>
+      <c r="D40" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E40" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F40" t="s">
+        <v>376</v>
+      </c>
+      <c r="G40">
+        <v>74</v>
+      </c>
+      <c r="H40" t="s">
+        <v>377</v>
+      </c>
+      <c r="I40">
+        <v>76</v>
+      </c>
+      <c r="J40" t="s">
+        <v>375</v>
+      </c>
+      <c r="K40">
+        <v>75</v>
+      </c>
+      <c r="L40" t="s">
+        <v>376</v>
+      </c>
+      <c r="M40">
+        <v>74</v>
+      </c>
+      <c r="N40">
+        <v>299</v>
+      </c>
+      <c r="O40">
+        <v>74.75</v>
+      </c>
+      <c r="P40">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="41" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B41" t="s">
+        <v>637</v>
+      </c>
+      <c r="C41" t="s">
+        <v>21</v>
+      </c>
+      <c r="D41" t="s">
+        <v>1154</v>
+      </c>
+      <c r="E41" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F41" t="s">
+        <v>376</v>
+      </c>
+      <c r="G41">
+        <v>74</v>
+      </c>
+      <c r="H41" t="s">
+        <v>374</v>
+      </c>
+      <c r="I41">
+        <v>77</v>
+      </c>
+      <c r="J41" t="s">
+        <v>376</v>
+      </c>
+      <c r="K41">
+        <v>74</v>
+      </c>
+      <c r="L41" t="s">
+        <v>377</v>
+      </c>
+      <c r="M41">
+        <v>74</v>
+      </c>
+      <c r="N41">
+        <v>299</v>
+      </c>
+      <c r="O41">
+        <v>74.75</v>
+      </c>
+      <c r="P41">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="42" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B42" t="s">
+        <v>662</v>
+      </c>
+      <c r="C42" t="s">
+        <v>21</v>
+      </c>
+      <c r="D42" t="s">
+        <v>1158</v>
+      </c>
+      <c r="E42" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F42" t="s">
+        <v>375</v>
+      </c>
+      <c r="G42">
+        <v>75</v>
+      </c>
+      <c r="H42" t="s">
+        <v>376</v>
+      </c>
+      <c r="I42">
+        <v>74</v>
+      </c>
+      <c r="J42" t="s">
+        <v>376</v>
+      </c>
+      <c r="K42">
+        <v>74</v>
+      </c>
+      <c r="L42" t="s">
+        <v>374</v>
+      </c>
+      <c r="M42">
+        <v>76</v>
+      </c>
+      <c r="N42">
+        <v>299</v>
+      </c>
+      <c r="O42">
+        <v>74.75</v>
+      </c>
+      <c r="P42">
+        <v>0.83</v>
+      </c>
+    </row>
+    <row r="43" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>1180</v>
+      </c>
+      <c r="B43" t="s">
+        <v>282</v>
+      </c>
+      <c r="C43" t="s">
+        <v>21</v>
+      </c>
+      <c r="D43" t="s">
+        <v>1153</v>
+      </c>
+      <c r="E43" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F43" t="s">
+        <v>375</v>
+      </c>
+      <c r="G43">
+        <v>73</v>
+      </c>
+      <c r="H43" t="s">
+        <v>374</v>
+      </c>
+      <c r="I43">
+        <v>78</v>
+      </c>
+      <c r="J43" t="s">
+        <v>376</v>
+      </c>
+      <c r="K43">
+        <v>74</v>
+      </c>
+      <c r="L43" t="s">
+        <v>375</v>
+      </c>
+      <c r="M43">
+        <v>74</v>
+      </c>
+      <c r="N43">
+        <v>299</v>
+      </c>
+      <c r="O43">
+        <v>74.75</v>
+      </c>
+      <c r="P43">
+        <v>1.92</v>
+      </c>
+    </row>
+    <row r="44" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>332</v>
+      </c>
+      <c r="B44" t="s">
+        <v>273</v>
+      </c>
+      <c r="C44" t="s">
+        <v>27</v>
+      </c>
+      <c r="D44" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E44" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F44" t="s">
+        <v>377</v>
+      </c>
+      <c r="G44">
+        <v>76</v>
+      </c>
+      <c r="H44" t="s">
+        <v>376</v>
+      </c>
+      <c r="I44">
+        <v>72</v>
+      </c>
+      <c r="J44" t="s">
+        <v>377</v>
+      </c>
+      <c r="K44">
+        <v>75</v>
+      </c>
+      <c r="L44" t="s">
+        <v>376</v>
+      </c>
+      <c r="M44">
+        <v>74</v>
+      </c>
+      <c r="N44">
+        <v>297</v>
+      </c>
+      <c r="O44">
+        <v>74.25</v>
+      </c>
+      <c r="P44">
+        <v>1.48</v>
+      </c>
+    </row>
+    <row r="45" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>332</v>
+      </c>
+      <c r="B45" t="s">
+        <v>696</v>
+      </c>
+      <c r="C45" t="s">
+        <v>21</v>
+      </c>
+      <c r="D45" t="s">
+        <v>1155</v>
+      </c>
+      <c r="E45" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F45" t="s">
+        <v>377</v>
+      </c>
+      <c r="G45">
+        <v>76</v>
+      </c>
+      <c r="H45" t="s">
+        <v>376</v>
+      </c>
+      <c r="I45">
+        <v>73</v>
+      </c>
+      <c r="J45" t="s">
+        <v>375</v>
+      </c>
+      <c r="K45">
+        <v>73</v>
+      </c>
+      <c r="L45" t="s">
+        <v>377</v>
+      </c>
+      <c r="M45">
+        <v>75</v>
+      </c>
+      <c r="N45">
+        <v>297</v>
+      </c>
+      <c r="O45">
+        <v>74.25</v>
+      </c>
+      <c r="P45">
+        <v>1.3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B46" t="s">
+        <v>1182</v>
+      </c>
+      <c r="C46" t="s">
+        <v>27</v>
+      </c>
+      <c r="D46" t="s">
+        <v>1161</v>
+      </c>
+      <c r="E46" t="s">
+        <v>1135</v>
+      </c>
+      <c r="F46" t="s">
+        <v>376</v>
+      </c>
+      <c r="G46">
+        <v>73</v>
+      </c>
+      <c r="H46" t="s">
+        <v>377</v>
+      </c>
+      <c r="I46">
+        <v>75</v>
+      </c>
+      <c r="J46" t="s">
+        <v>375</v>
+      </c>
+      <c r="K46">
+        <v>75</v>
+      </c>
+      <c r="L46" t="s">
+        <v>376</v>
+      </c>
+      <c r="M46">
+        <v>73</v>
+      </c>
+      <c r="N46">
+        <v>296</v>
+      </c>
+      <c r="O46">
+        <v>74</v>
+      </c>
+      <c r="P46">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B47" t="s">
+        <v>276</v>
+      </c>
+      <c r="C47" t="s">
+        <v>27</v>
+      </c>
+      <c r="D47" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E47" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F47" t="s">
+        <v>376</v>
+      </c>
+      <c r="G47">
+        <v>72</v>
+      </c>
+      <c r="H47" t="s">
+        <v>376</v>
+      </c>
+      <c r="I47">
+        <v>74</v>
+      </c>
+      <c r="J47" t="s">
+        <v>375</v>
+      </c>
+      <c r="K47">
+        <v>75</v>
+      </c>
+      <c r="L47" t="s">
+        <v>376</v>
+      </c>
+      <c r="M47">
+        <v>75</v>
+      </c>
+      <c r="N47">
+        <v>296</v>
+      </c>
+      <c r="O47">
+        <v>74</v>
+      </c>
+      <c r="P47">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="48" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>1181</v>
+      </c>
+      <c r="B48" t="s">
+        <v>287</v>
+      </c>
+      <c r="C48" t="s">
+        <v>27</v>
+      </c>
+      <c r="D48" t="s">
+        <v>1159</v>
+      </c>
+      <c r="E48" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F48" t="s">
+        <v>377</v>
+      </c>
+      <c r="G48">
+        <v>74</v>
+      </c>
+      <c r="H48" t="s">
+        <v>376</v>
+      </c>
+      <c r="I48">
+        <v>73</v>
+      </c>
+      <c r="J48" t="s">
+        <v>377</v>
+      </c>
+      <c r="K48">
+        <v>76</v>
+      </c>
+      <c r="L48" t="s">
+        <v>376</v>
+      </c>
+      <c r="M48">
+        <v>73</v>
+      </c>
+      <c r="N48">
+        <v>296</v>
+      </c>
+      <c r="O48">
+        <v>74</v>
+      </c>
+      <c r="P48">
+        <v>1.22</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.35">
+      <c r="A49">
+        <v>48</v>
+      </c>
+      <c r="B49" t="s">
+        <v>275</v>
+      </c>
+      <c r="C49" t="s">
+        <v>27</v>
+      </c>
+      <c r="D49" t="s">
+        <v>1162</v>
+      </c>
+      <c r="E49" t="s">
+        <v>1138</v>
+      </c>
+      <c r="F49" t="s">
+        <v>376</v>
+      </c>
+      <c r="G49">
+        <v>70</v>
+      </c>
+      <c r="H49" t="s">
+        <v>376</v>
+      </c>
+      <c r="I49">
+        <v>74</v>
+      </c>
+      <c r="J49" t="s">
+        <v>375</v>
+      </c>
+      <c r="K49">
+        <v>75</v>
+      </c>
+      <c r="L49" t="s">
+        <v>376</v>
+      </c>
+      <c r="M49">
+        <v>74</v>
+      </c>
+      <c r="N49">
+        <v>293</v>
+      </c>
+      <c r="O49">
+        <v>73.25</v>
+      </c>
+      <c r="P49">
+        <v>1.92</v>
       </c>
     </row>
   </sheetData>
-  <hyperlinks>
-    <hyperlink ref="A1" r:id="rId1" xr:uid="{5C4DE4E2-D020-498A-A941-2A23105AB5D9}"/>
-  </hyperlinks>
+  <sortState xmlns:xlrd2="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata2" ref="R2:AC25">
+    <sortCondition ref="S2:S25"/>
+  </sortState>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -14718,7 +17313,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{521D9E93-0418-4A29-ADAE-6AFF0EAB4B20}">
   <dimension ref="A1:Q97"/>
   <sheetViews>
-    <sheetView topLeftCell="J1" zoomScale="105" workbookViewId="0">
+    <sheetView zoomScale="105" workbookViewId="0">
       <selection activeCell="U14" sqref="U14"/>
     </sheetView>
   </sheetViews>
@@ -19750,7 +22345,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D5F9ABE-3119-480D-8EBD-CC89A58F8F56}">
   <dimension ref="A1:R177"/>
   <sheetViews>
-    <sheetView topLeftCell="P1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="G6" sqref="G6"/>
     </sheetView>
   </sheetViews>
@@ -29681,7 +32276,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2742109F-5A5B-4C32-91D0-D2232F8832B6}">
   <dimension ref="A1:Q284"/>
   <sheetViews>
-    <sheetView topLeftCell="O1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="R1" sqref="R1"/>
     </sheetView>
   </sheetViews>
@@ -44403,4 +46998,25 @@
   <sheetData/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{69662653-AB67-4ED4-84CD-11BED4B53108}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.35">
+      <c r="A1" s="1" t="s">
+        <v>537</v>
+      </c>
+    </row>
+  </sheetData>
+  <hyperlinks>
+    <hyperlink ref="A1" r:id="rId1" xr:uid="{49F2BAD1-6018-45F8-A385-506D33BBE769}"/>
+  </hyperlinks>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>